<commit_message>
initial addition of methylated histones working, rate of methylation equal at 0.001
</commit_message>
<xml_diff>
--- a/chromatin_model.xlsx
+++ b/chromatin_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Allison/Box Sync/ABS/UCLA/+1 First Year/Hoffmann-Fall/ModelingProject/ksheu.library2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44401D2B-1C1E-EE49-BB18-72A235C450DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3D9581-611D-1848-B3F7-B53817FE5382}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="480" windowWidth="23000" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="23000" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="6" r:id="rId1"/>
@@ -275,6 +275,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -413,6 +416,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
@@ -3260,7 +3264,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3525,8 +3529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G129" sqref="G129"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113:E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4884,7 +4888,7 @@
     </row>
     <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>61</v>
@@ -4953,7 +4957,7 @@
     </row>
     <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="13">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B61" s="14" t="s">
         <v>47</v>
@@ -4978,7 +4982,7 @@
     </row>
     <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>62</v>
@@ -5048,7 +5052,7 @@
     </row>
     <row r="65" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="13">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>48</v>
@@ -5074,7 +5078,7 @@
     </row>
     <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>63</v>
@@ -5144,7 +5148,7 @@
     </row>
     <row r="69" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="13">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B69" s="14" t="s">
         <v>49</v>
@@ -5170,7 +5174,7 @@
     </row>
     <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>64</v>
@@ -5240,7 +5244,7 @@
     </row>
     <row r="73" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="13">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B73" s="14" t="s">
         <v>50</v>
@@ -5266,7 +5270,7 @@
     </row>
     <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>65</v>
@@ -5336,7 +5340,7 @@
     </row>
     <row r="77" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="13">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B77" s="14" t="s">
         <v>51</v>
@@ -5362,7 +5366,7 @@
     </row>
     <row r="78" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>66</v>
@@ -5432,7 +5436,7 @@
     </row>
     <row r="81" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="13">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B81" s="14" t="s">
         <v>52</v>
@@ -5458,7 +5462,7 @@
     </row>
     <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>67</v>
@@ -5528,7 +5532,7 @@
     </row>
     <row r="85" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="13">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B85" s="14" t="s">
         <v>53</v>
@@ -5554,7 +5558,7 @@
     </row>
     <row r="86" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>68</v>
@@ -5624,7 +5628,7 @@
     </row>
     <row r="89" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="13">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B89" s="14" t="s">
         <v>54</v>
@@ -5650,7 +5654,7 @@
     </row>
     <row r="90" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>69</v>
@@ -5720,7 +5724,7 @@
     </row>
     <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="13">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B93" s="14" t="s">
         <v>55</v>
@@ -5746,7 +5750,7 @@
     </row>
     <row r="94" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>70</v>
@@ -5816,7 +5820,7 @@
     </row>
     <row r="97" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="13">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B97" s="14" t="s">
         <v>56</v>
@@ -5842,7 +5846,7 @@
     </row>
     <row r="98" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>71</v>
@@ -5912,7 +5916,7 @@
     </row>
     <row r="101" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="13">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B101" s="14" t="s">
         <v>57</v>
@@ -5938,7 +5942,7 @@
     </row>
     <row r="102" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>72</v>
@@ -6008,7 +6012,7 @@
     </row>
     <row r="105" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="13">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B105" s="14" t="s">
         <v>58</v>
@@ -6034,7 +6038,7 @@
     </row>
     <row r="106" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>73</v>
@@ -6104,7 +6108,7 @@
     </row>
     <row r="109" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="13">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B109" s="14" t="s">
         <v>59</v>
@@ -6130,7 +6134,7 @@
     </row>
     <row r="110" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>74</v>
@@ -6200,7 +6204,7 @@
     </row>
     <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B113" t="s">
         <v>10</v>
@@ -6211,8 +6215,8 @@
       <c r="D113" t="s">
         <v>46</v>
       </c>
-      <c r="E113" s="20">
-        <v>1</v>
+      <c r="E113" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F113" t="s">
         <v>24</v>
@@ -6223,7 +6227,7 @@
     </row>
     <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B114" t="s">
         <v>11</v>
@@ -6234,8 +6238,8 @@
       <c r="D114" t="s">
         <v>47</v>
       </c>
-      <c r="E114" s="20">
-        <v>1</v>
+      <c r="E114" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F114" t="s">
         <v>24</v>
@@ -6246,7 +6250,7 @@
     </row>
     <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B115" t="s">
         <v>12</v>
@@ -6257,8 +6261,8 @@
       <c r="D115" t="s">
         <v>48</v>
       </c>
-      <c r="E115" s="20">
-        <v>1</v>
+      <c r="E115" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F115" t="s">
         <v>24</v>
@@ -6269,7 +6273,7 @@
     </row>
     <row r="116" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B116" t="s">
         <v>13</v>
@@ -6280,8 +6284,8 @@
       <c r="D116" t="s">
         <v>49</v>
       </c>
-      <c r="E116" s="20">
-        <v>1</v>
+      <c r="E116" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F116" t="s">
         <v>24</v>
@@ -6292,7 +6296,7 @@
     </row>
     <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B117" t="s">
         <v>14</v>
@@ -6303,8 +6307,8 @@
       <c r="D117" t="s">
         <v>50</v>
       </c>
-      <c r="E117" s="20">
-        <v>1</v>
+      <c r="E117" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F117" t="s">
         <v>24</v>
@@ -6315,7 +6319,7 @@
     </row>
     <row r="118" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B118" t="s">
         <v>15</v>
@@ -6326,8 +6330,8 @@
       <c r="D118" t="s">
         <v>51</v>
       </c>
-      <c r="E118" s="20">
-        <v>1</v>
+      <c r="E118" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F118" t="s">
         <v>24</v>
@@ -6338,7 +6342,7 @@
     </row>
     <row r="119" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B119" t="s">
         <v>16</v>
@@ -6349,8 +6353,8 @@
       <c r="D119" t="s">
         <v>52</v>
       </c>
-      <c r="E119" s="20">
-        <v>1</v>
+      <c r="E119" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F119" t="s">
         <v>24</v>
@@ -6361,7 +6365,7 @@
     </row>
     <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B120" t="s">
         <v>17</v>
@@ -6372,8 +6376,8 @@
       <c r="D120" t="s">
         <v>53</v>
       </c>
-      <c r="E120" s="20">
-        <v>1</v>
+      <c r="E120" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F120" t="s">
         <v>24</v>
@@ -6384,7 +6388,7 @@
     </row>
     <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B121" t="s">
         <v>18</v>
@@ -6395,8 +6399,8 @@
       <c r="D121" t="s">
         <v>54</v>
       </c>
-      <c r="E121" s="20">
-        <v>1</v>
+      <c r="E121" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F121" t="s">
         <v>24</v>
@@ -6407,7 +6411,7 @@
     </row>
     <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B122" t="s">
         <v>19</v>
@@ -6418,8 +6422,8 @@
       <c r="D122" t="s">
         <v>55</v>
       </c>
-      <c r="E122" s="20">
-        <v>1</v>
+      <c r="E122" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F122" t="s">
         <v>24</v>
@@ -6430,7 +6434,7 @@
     </row>
     <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B123" t="s">
         <v>20</v>
@@ -6441,8 +6445,8 @@
       <c r="D123" t="s">
         <v>56</v>
       </c>
-      <c r="E123" s="20">
-        <v>1</v>
+      <c r="E123" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F123" t="s">
         <v>24</v>
@@ -6453,7 +6457,7 @@
     </row>
     <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B124" t="s">
         <v>21</v>
@@ -6464,8 +6468,8 @@
       <c r="D124" t="s">
         <v>57</v>
       </c>
-      <c r="E124" s="20">
-        <v>1</v>
+      <c r="E124" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F124" t="s">
         <v>24</v>
@@ -6476,7 +6480,7 @@
     </row>
     <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B125" t="s">
         <v>22</v>
@@ -6487,8 +6491,8 @@
       <c r="D125" t="s">
         <v>58</v>
       </c>
-      <c r="E125" s="20">
-        <v>1</v>
+      <c r="E125" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F125" t="s">
         <v>24</v>
@@ -6499,7 +6503,7 @@
     </row>
     <row r="126" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B126" t="s">
         <v>23</v>
@@ -6510,8 +6514,8 @@
       <c r="D126" t="s">
         <v>59</v>
       </c>
-      <c r="E126" s="20">
-        <v>1</v>
+      <c r="E126" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F126" t="s">
         <v>24</v>
@@ -6522,7 +6526,7 @@
     </row>
     <row r="127" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B127" t="s">
         <v>30</v>
@@ -6533,8 +6537,8 @@
       <c r="D127" t="s">
         <v>60</v>
       </c>
-      <c r="E127" s="20">
-        <v>1</v>
+      <c r="E127" s="24">
+        <v>1E-3</v>
       </c>
       <c r="F127" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
fixed missing ODE in excel sheet
</commit_message>
<xml_diff>
--- a/chromatin_model.xlsx
+++ b/chromatin_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Allison/Box Sync/ABS/UCLA/+1 First Year/Hoffmann-Fall/ModelingProject/ksheu.library2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3D9581-611D-1848-B3F7-B53817FE5382}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A343B64F-B0BC-6449-A64B-A8469B73F494}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="460" windowWidth="23000" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="460" windowWidth="23540" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="76">
   <si>
     <t>#</t>
   </si>
@@ -422,7 +422,7 @@
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="183">
+  <dxfs count="182">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1421,6 +1421,20 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
@@ -1435,6 +1449,34 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
@@ -1449,34 +1491,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
@@ -1645,6 +1659,34 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
@@ -2150,62 +2192,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
       <border>
@@ -3527,10 +3513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113:E127"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E114" sqref="E114:E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6202,44 +6188,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113">
+    <row r="113" spans="1:9" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="13">
         <v>56</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E113" s="12">
+        <f>E109*0.8</f>
+        <v>4.1231686041600035</v>
+      </c>
+      <c r="F113" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G113" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H113" s="17"/>
+      <c r="I113" s="17"/>
+    </row>
+    <row r="114" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="13">
+        <v>57</v>
+      </c>
+      <c r="B114" t="s">
         <v>10</v>
       </c>
-      <c r="C113" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="C114" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" t="s">
         <v>46</v>
       </c>
-      <c r="E113" s="24">
-        <v>1E-3</v>
-      </c>
-      <c r="F113" t="s">
-        <v>24</v>
-      </c>
-      <c r="G113" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114">
-        <v>57</v>
-      </c>
-      <c r="B114" t="s">
-        <v>11</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" t="s">
-        <v>47</v>
-      </c>
       <c r="E114" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F114" t="s">
         <v>24</v>
@@ -6248,21 +6237,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115">
+    <row r="115" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="13">
         <v>58</v>
       </c>
       <c r="B115" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E115" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F115" t="s">
         <v>24</v>
@@ -6271,21 +6260,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116">
+    <row r="116" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="13">
         <v>59</v>
       </c>
       <c r="B116" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E116" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F116" t="s">
         <v>24</v>
@@ -6294,21 +6283,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117">
+    <row r="117" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="13">
         <v>60</v>
       </c>
       <c r="B117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E117" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F117" t="s">
         <v>24</v>
@@ -6317,21 +6306,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118">
+    <row r="118" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="13">
         <v>61</v>
       </c>
       <c r="B118" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E118" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F118" t="s">
         <v>24</v>
@@ -6340,21 +6329,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119">
+    <row r="119" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="13">
         <v>62</v>
       </c>
       <c r="B119" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E119" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F119" t="s">
         <v>24</v>
@@ -6363,21 +6352,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120">
+    <row r="120" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="13">
         <v>63</v>
       </c>
       <c r="B120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E120" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F120" t="s">
         <v>24</v>
@@ -6386,21 +6375,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121">
+    <row r="121" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="13">
         <v>64</v>
       </c>
       <c r="B121" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E121" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F121" t="s">
         <v>24</v>
@@ -6409,21 +6398,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122">
+    <row r="122" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="13">
         <v>65</v>
       </c>
       <c r="B122" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E122" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F122" t="s">
         <v>24</v>
@@ -6432,21 +6421,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123">
+    <row r="123" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="13">
         <v>66</v>
       </c>
       <c r="B123" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E123" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F123" t="s">
         <v>24</v>
@@ -6455,21 +6444,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124">
+    <row r="124" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="13">
         <v>67</v>
       </c>
       <c r="B124" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E124" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F124" t="s">
         <v>24</v>
@@ -6478,21 +6467,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125">
+    <row r="125" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="13">
         <v>68</v>
       </c>
       <c r="B125" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E125" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F125" t="s">
         <v>24</v>
@@ -6501,21 +6490,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126">
+    <row r="126" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="13">
         <v>69</v>
       </c>
       <c r="B126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E126" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F126" t="s">
         <v>24</v>
@@ -6524,26 +6513,49 @@
         <v>75</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127">
+    <row r="127" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="13">
         <v>70</v>
       </c>
       <c r="B127" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E127" s="24">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F127" t="s">
         <v>24</v>
       </c>
       <c r="G127" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="13">
+        <v>71</v>
+      </c>
+      <c r="B128" t="s">
+        <v>30</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" t="s">
+        <v>60</v>
+      </c>
+      <c r="E128" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="F128" t="s">
+        <v>24</v>
+      </c>
+      <c r="G128" s="23" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6580,38 +6592,33 @@
     <mergeCell ref="A18:A20"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:D2 C5:D5 C9 C13 C17 C21 C25 C29 C33 C37 C41 C45 C49 C53">
-    <cfRule type="expression" dxfId="182" priority="114">
-      <formula>ISODD($K2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:D2">
     <cfRule type="expression" dxfId="181" priority="115">
       <formula>ISODD($K2)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C2:D2">
+    <cfRule type="expression" dxfId="180" priority="116">
+      <formula>ISODD($K2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3:I4 E7:I8 E11:I12 E15:I16 E19:I20 E23:I24 E27:I28 E31:I32 E35:I36 E39:I40 E43:I44 E47:I48 E51:I52 E55:I56">
-    <cfRule type="expression" dxfId="180" priority="113">
+    <cfRule type="expression" dxfId="179" priority="114">
       <formula>ISODD($I3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="179" priority="110">
+    <cfRule type="expression" dxfId="178" priority="111">
       <formula>ISODD($K6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="178" priority="109">
+    <cfRule type="expression" dxfId="177" priority="110">
       <formula>ISODD($K6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:C8">
-    <cfRule type="expression" dxfId="177" priority="108">
+    <cfRule type="expression" dxfId="176" priority="109">
       <formula>ISODD($I7)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="176" priority="106">
-      <formula>ISODD($K10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
@@ -6619,14 +6626,14 @@
       <formula>ISODD($K10)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="174" priority="108">
+      <formula>ISODD($K10)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B11:C12">
-    <cfRule type="expression" dxfId="174" priority="105">
+    <cfRule type="expression" dxfId="173" priority="106">
       <formula>ISODD($I11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="173" priority="103">
-      <formula>ISODD($K14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
@@ -6634,14 +6641,14 @@
       <formula>ISODD($K14)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="171" priority="105">
+      <formula>ISODD($K14)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B15:C16">
-    <cfRule type="expression" dxfId="171" priority="102">
+    <cfRule type="expression" dxfId="170" priority="103">
       <formula>ISODD($I15)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="170" priority="100">
-      <formula>ISODD($K18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
@@ -6649,14 +6656,14 @@
       <formula>ISODD($K18)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="168" priority="102">
+      <formula>ISODD($K18)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B19:C20">
-    <cfRule type="expression" dxfId="168" priority="99">
+    <cfRule type="expression" dxfId="167" priority="100">
       <formula>ISODD($I19)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="167" priority="97">
-      <formula>ISODD($K22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
@@ -6664,14 +6671,14 @@
       <formula>ISODD($K22)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="165" priority="99">
+      <formula>ISODD($K22)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B23:C24">
-    <cfRule type="expression" dxfId="165" priority="96">
+    <cfRule type="expression" dxfId="164" priority="97">
       <formula>ISODD($I23)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="164" priority="94">
-      <formula>ISODD($K26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
@@ -6679,14 +6686,14 @@
       <formula>ISODD($K26)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="162" priority="96">
+      <formula>ISODD($K26)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B27:C28">
-    <cfRule type="expression" dxfId="162" priority="93">
+    <cfRule type="expression" dxfId="161" priority="94">
       <formula>ISODD($I27)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="161" priority="91">
-      <formula>ISODD($K30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
@@ -6694,14 +6701,14 @@
       <formula>ISODD($K30)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="159" priority="93">
+      <formula>ISODD($K30)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B31:C32">
-    <cfRule type="expression" dxfId="159" priority="90">
+    <cfRule type="expression" dxfId="158" priority="91">
       <formula>ISODD($I31)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="158" priority="88">
-      <formula>ISODD($K34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
@@ -6709,14 +6716,14 @@
       <formula>ISODD($K34)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="156" priority="90">
+      <formula>ISODD($K34)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B35:C36">
-    <cfRule type="expression" dxfId="156" priority="87">
+    <cfRule type="expression" dxfId="155" priority="88">
       <formula>ISODD($I35)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="155" priority="85">
-      <formula>ISODD($K38)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
@@ -6724,14 +6731,14 @@
       <formula>ISODD($K38)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="153" priority="87">
+      <formula>ISODD($K38)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B39:C40">
-    <cfRule type="expression" dxfId="153" priority="84">
+    <cfRule type="expression" dxfId="152" priority="85">
       <formula>ISODD($I39)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="152" priority="82">
-      <formula>ISODD($K42)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
@@ -6739,14 +6746,14 @@
       <formula>ISODD($K42)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="150" priority="84">
+      <formula>ISODD($K42)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B43:C44">
-    <cfRule type="expression" dxfId="150" priority="81">
+    <cfRule type="expression" dxfId="149" priority="82">
       <formula>ISODD($I43)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="149" priority="79">
-      <formula>ISODD($K46)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
@@ -6754,14 +6761,14 @@
       <formula>ISODD($K46)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="147" priority="81">
+      <formula>ISODD($K46)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B47:C48">
-    <cfRule type="expression" dxfId="147" priority="78">
+    <cfRule type="expression" dxfId="146" priority="79">
       <formula>ISODD($I47)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="146" priority="76">
-      <formula>ISODD($K50)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
@@ -6769,74 +6776,74 @@
       <formula>ISODD($K50)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="144" priority="78">
+      <formula>ISODD($K50)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B51:C52">
-    <cfRule type="expression" dxfId="144" priority="75">
+    <cfRule type="expression" dxfId="143" priority="76">
       <formula>ISODD($I51)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8">
-    <cfRule type="expression" dxfId="143" priority="74">
+    <cfRule type="expression" dxfId="142" priority="75">
       <formula>ISODD($I7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D12">
-    <cfRule type="expression" dxfId="142" priority="73">
+    <cfRule type="expression" dxfId="141" priority="74">
       <formula>ISODD($I11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D16">
-    <cfRule type="expression" dxfId="141" priority="72">
+    <cfRule type="expression" dxfId="140" priority="73">
       <formula>ISODD($I15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:D20">
-    <cfRule type="expression" dxfId="140" priority="71">
+    <cfRule type="expression" dxfId="139" priority="72">
       <formula>ISODD($I19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="expression" dxfId="139" priority="70">
+    <cfRule type="expression" dxfId="138" priority="71">
       <formula>ISODD($I23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D28">
-    <cfRule type="expression" dxfId="138" priority="69">
+    <cfRule type="expression" dxfId="137" priority="70">
       <formula>ISODD($I27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D32">
-    <cfRule type="expression" dxfId="137" priority="68">
+    <cfRule type="expression" dxfId="136" priority="69">
       <formula>ISODD($I31)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D36">
-    <cfRule type="expression" dxfId="136" priority="67">
+    <cfRule type="expression" dxfId="135" priority="68">
       <formula>ISODD($I35)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:D40">
-    <cfRule type="expression" dxfId="135" priority="66">
+    <cfRule type="expression" dxfId="134" priority="67">
       <formula>ISODD($I39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D44">
-    <cfRule type="expression" dxfId="134" priority="65">
+    <cfRule type="expression" dxfId="133" priority="66">
       <formula>ISODD($I43)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47:D48">
-    <cfRule type="expression" dxfId="133" priority="64">
+    <cfRule type="expression" dxfId="132" priority="65">
       <formula>ISODD($I47)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D52">
-    <cfRule type="expression" dxfId="132" priority="63">
+    <cfRule type="expression" dxfId="131" priority="64">
       <formula>ISODD($I51)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="131" priority="61">
-      <formula>ISODD($K54)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
@@ -6844,288 +6851,293 @@
       <formula>ISODD($K54)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="129" priority="63">
+      <formula>ISODD($K54)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B55:C56">
-    <cfRule type="expression" dxfId="129" priority="60">
+    <cfRule type="expression" dxfId="128" priority="61">
       <formula>ISODD($I55)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:D56">
-    <cfRule type="expression" dxfId="128" priority="59">
+    <cfRule type="expression" dxfId="127" priority="60">
       <formula>ISODD($I55)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111:D112">
-    <cfRule type="expression" dxfId="126" priority="2">
+    <cfRule type="expression" dxfId="126" priority="3">
       <formula>ISODD($I111)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:D58 C61:D61 C65 C69 C73 C77 C81 C85 C89 C93 C97 C101 C105 C109">
-    <cfRule type="expression" dxfId="125" priority="55">
+    <cfRule type="expression" dxfId="125" priority="56">
       <formula>ISODD($K58)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:D58">
-    <cfRule type="expression" dxfId="124" priority="56">
+    <cfRule type="expression" dxfId="124" priority="57">
       <formula>ISODD($K58)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59:I60 E63:I64 E67:I68 E71:I72 E75:I76 E79:I80 E83:I84 E87:I88 E91:I92 E95:I96 E99:I100 E103:I104 E107:I108 E111:I112 G113:G127">
-    <cfRule type="expression" dxfId="123" priority="54">
+  <conditionalFormatting sqref="B59:I60 E63:I64 E67:I68 E71:I72 E75:I76 E79:I80 E83:I84 E87:I88 E91:I92 E95:I96 E99:I100 E103:I104 E107:I108 E111:I112 G114:G128">
+    <cfRule type="expression" dxfId="123" priority="55">
       <formula>ISODD($I59)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="122" priority="53">
+    <cfRule type="expression" dxfId="122" priority="54">
       <formula>ISODD($K62)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="121" priority="52">
+    <cfRule type="expression" dxfId="121" priority="53">
       <formula>ISODD($K62)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:C64">
-    <cfRule type="expression" dxfId="120" priority="51">
+    <cfRule type="expression" dxfId="120" priority="52">
       <formula>ISODD($I63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="119" priority="49">
+    <cfRule type="expression" dxfId="119" priority="50">
       <formula>ISODD($K66)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="118" priority="50">
+    <cfRule type="expression" dxfId="118" priority="51">
       <formula>ISODD($K66)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67:C68">
-    <cfRule type="expression" dxfId="117" priority="48">
+    <cfRule type="expression" dxfId="117" priority="49">
       <formula>ISODD($I67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="116" priority="46">
+    <cfRule type="expression" dxfId="116" priority="47">
       <formula>ISODD($K70)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="115" priority="47">
+    <cfRule type="expression" dxfId="115" priority="48">
       <formula>ISODD($K70)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71:C72">
-    <cfRule type="expression" dxfId="114" priority="45">
+    <cfRule type="expression" dxfId="114" priority="46">
       <formula>ISODD($I71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="113" priority="43">
+    <cfRule type="expression" dxfId="113" priority="44">
       <formula>ISODD($K74)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="expression" dxfId="112" priority="44">
+    <cfRule type="expression" dxfId="112" priority="45">
       <formula>ISODD($K74)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:C76">
-    <cfRule type="expression" dxfId="111" priority="42">
+    <cfRule type="expression" dxfId="111" priority="43">
       <formula>ISODD($I75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="expression" dxfId="110" priority="40">
+    <cfRule type="expression" dxfId="110" priority="41">
       <formula>ISODD($K78)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="expression" dxfId="109" priority="41">
+    <cfRule type="expression" dxfId="109" priority="42">
       <formula>ISODD($K78)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79:C80">
-    <cfRule type="expression" dxfId="108" priority="39">
+    <cfRule type="expression" dxfId="108" priority="40">
       <formula>ISODD($I79)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82">
-    <cfRule type="expression" dxfId="107" priority="37">
+    <cfRule type="expression" dxfId="107" priority="38">
       <formula>ISODD($K82)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82">
-    <cfRule type="expression" dxfId="106" priority="38">
+    <cfRule type="expression" dxfId="106" priority="39">
       <formula>ISODD($K82)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:C84">
-    <cfRule type="expression" dxfId="105" priority="36">
+    <cfRule type="expression" dxfId="105" priority="37">
       <formula>ISODD($I83)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="expression" dxfId="104" priority="34">
+    <cfRule type="expression" dxfId="104" priority="35">
       <formula>ISODD($K86)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="expression" dxfId="103" priority="35">
+    <cfRule type="expression" dxfId="103" priority="36">
       <formula>ISODD($K86)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87:C88">
-    <cfRule type="expression" dxfId="102" priority="33">
+    <cfRule type="expression" dxfId="102" priority="34">
       <formula>ISODD($I87)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="101" priority="31">
+    <cfRule type="expression" dxfId="101" priority="32">
       <formula>ISODD($K90)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="100" priority="32">
+    <cfRule type="expression" dxfId="100" priority="33">
       <formula>ISODD($K90)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91:C92">
-    <cfRule type="expression" dxfId="99" priority="30">
+    <cfRule type="expression" dxfId="99" priority="31">
       <formula>ISODD($I91)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
-    <cfRule type="expression" dxfId="98" priority="28">
+    <cfRule type="expression" dxfId="98" priority="29">
       <formula>ISODD($K94)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
-    <cfRule type="expression" dxfId="97" priority="29">
+    <cfRule type="expression" dxfId="97" priority="30">
       <formula>ISODD($K94)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95:C96">
-    <cfRule type="expression" dxfId="96" priority="27">
+    <cfRule type="expression" dxfId="96" priority="28">
       <formula>ISODD($I95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="expression" dxfId="95" priority="25">
+    <cfRule type="expression" dxfId="95" priority="26">
       <formula>ISODD($K98)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="expression" dxfId="94" priority="26">
+    <cfRule type="expression" dxfId="94" priority="27">
       <formula>ISODD($K98)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99:C100">
-    <cfRule type="expression" dxfId="93" priority="24">
+    <cfRule type="expression" dxfId="93" priority="25">
       <formula>ISODD($I99)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
-    <cfRule type="expression" dxfId="92" priority="22">
+    <cfRule type="expression" dxfId="92" priority="23">
       <formula>ISODD($K102)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102">
-    <cfRule type="expression" dxfId="91" priority="23">
+    <cfRule type="expression" dxfId="91" priority="24">
       <formula>ISODD($K102)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B103:C104">
-    <cfRule type="expression" dxfId="90" priority="21">
+    <cfRule type="expression" dxfId="90" priority="22">
       <formula>ISODD($I103)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="89" priority="19">
+    <cfRule type="expression" dxfId="89" priority="20">
       <formula>ISODD($K106)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106">
-    <cfRule type="expression" dxfId="88" priority="20">
+    <cfRule type="expression" dxfId="88" priority="21">
       <formula>ISODD($K106)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B107:C108">
-    <cfRule type="expression" dxfId="87" priority="18">
+    <cfRule type="expression" dxfId="87" priority="19">
       <formula>ISODD($I107)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:D64">
-    <cfRule type="expression" dxfId="86" priority="17">
+    <cfRule type="expression" dxfId="86" priority="18">
       <formula>ISODD($I63)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67:D68">
-    <cfRule type="expression" dxfId="85" priority="16">
+    <cfRule type="expression" dxfId="85" priority="17">
       <formula>ISODD($I67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:D72">
-    <cfRule type="expression" dxfId="84" priority="15">
+    <cfRule type="expression" dxfId="84" priority="16">
       <formula>ISODD($I71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75:D76">
-    <cfRule type="expression" dxfId="83" priority="14">
+    <cfRule type="expression" dxfId="83" priority="15">
       <formula>ISODD($I75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79:D80">
-    <cfRule type="expression" dxfId="82" priority="13">
+    <cfRule type="expression" dxfId="82" priority="14">
       <formula>ISODD($I79)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:D84">
-    <cfRule type="expression" dxfId="81" priority="12">
+    <cfRule type="expression" dxfId="81" priority="13">
       <formula>ISODD($I83)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87:D88">
-    <cfRule type="expression" dxfId="80" priority="11">
+    <cfRule type="expression" dxfId="80" priority="12">
       <formula>ISODD($I87)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91:D92">
-    <cfRule type="expression" dxfId="79" priority="10">
+    <cfRule type="expression" dxfId="79" priority="11">
       <formula>ISODD($I91)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D95:D96">
-    <cfRule type="expression" dxfId="78" priority="9">
+    <cfRule type="expression" dxfId="78" priority="10">
       <formula>ISODD($I95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D99:D100">
-    <cfRule type="expression" dxfId="77" priority="8">
+    <cfRule type="expression" dxfId="77" priority="9">
       <formula>ISODD($I99)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103:D104">
-    <cfRule type="expression" dxfId="76" priority="7">
+    <cfRule type="expression" dxfId="76" priority="8">
       <formula>ISODD($I103)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D107:D108">
-    <cfRule type="expression" dxfId="75" priority="6">
+    <cfRule type="expression" dxfId="75" priority="7">
       <formula>ISODD($I107)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C110">
-    <cfRule type="expression" dxfId="74" priority="4">
+    <cfRule type="expression" dxfId="74" priority="5">
       <formula>ISODD($K110)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C110">
-    <cfRule type="expression" dxfId="73" priority="5">
+    <cfRule type="expression" dxfId="73" priority="6">
       <formula>ISODD($K110)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B111:C112 C113:C127">
-    <cfRule type="expression" dxfId="72" priority="3">
+  <conditionalFormatting sqref="B111:C112 C114:C128">
+    <cfRule type="expression" dxfId="72" priority="4">
       <formula>ISODD($I111)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7135,7 +7147,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{4CE0990A-53FF-3C4E-B908-CE9F7EFAFE49}">
+          <x14:cfRule type="expression" priority="2" id="{4CE0990A-53FF-3C4E-B908-CE9F7EFAFE49}">
             <xm:f>ISODD('Reactions-2'!$K57)</xm:f>
             <x14:dxf>
               <fill>
@@ -7153,6 +7165,26 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>C57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{A6D7B81E-F551-904F-9A9A-9B4F90F81E0A}">
+            <xm:f>ISODD('Reactions-2'!$K113)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFF3F3F3"/>
+                  <bgColor rgb="FFF3F3F3"/>
+                </patternFill>
+              </fill>
+              <border>
+                <left/>
+                <right/>
+                <top/>
+                <bottom/>
+              </border>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C113</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
went back to d3d785c9a to make sure I didn't actually change anything
</commit_message>
<xml_diff>
--- a/chromatin_model.xlsx
+++ b/chromatin_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Allison/Box Sync/ABS/UCLA/+1 First Year/Hoffmann-Fall/ModelingProject/ksheu.library2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A343B64F-B0BC-6449-A64B-A8469B73F494}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2FE73F-4E4C-EF42-89C9-7084ADF6FDD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="460" windowWidth="23540" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="460" windowWidth="23540" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="6" r:id="rId1"/>
@@ -276,7 +276,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -410,13 +410,13 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
@@ -427,20 +427,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
@@ -1380,6 +1366,20 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
       <border>
@@ -3515,8 +3515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114:E128"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115:E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3557,7 +3557,7 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="22">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -3582,7 +3582,7 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="22"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -3604,7 +3604,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -3649,7 +3649,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="24">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3675,7 +3675,7 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -3697,7 +3697,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -3743,7 +3743,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="22">
+      <c r="A10" s="24">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -3769,7 +3769,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="22"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>6</v>
@@ -3791,7 +3791,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="22"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>6</v>
@@ -3837,7 +3837,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
+      <c r="A14" s="24">
         <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -3863,7 +3863,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="22"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
         <v>6</v>
@@ -3885,7 +3885,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="22"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>6</v>
@@ -3931,7 +3931,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="22">
+      <c r="A18" s="24">
         <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -3957,7 +3957,7 @@
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="22"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>6</v>
@@ -3979,7 +3979,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="22"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
         <v>6</v>
@@ -4025,7 +4025,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="22">
+      <c r="A22" s="24">
         <v>11</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -4051,7 +4051,7 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="22"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="s">
         <v>6</v>
@@ -4073,7 +4073,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="22"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
         <v>6</v>
@@ -4119,7 +4119,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="22">
+      <c r="A26" s="24">
         <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -4145,7 +4145,7 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="22"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>6</v>
@@ -4167,7 +4167,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="22"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
         <v>6</v>
@@ -4213,7 +4213,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="22">
+      <c r="A30" s="24">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -4239,7 +4239,7 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="22"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
         <v>6</v>
@@ -4261,7 +4261,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="22"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
         <v>6</v>
@@ -4307,7 +4307,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="22">
+      <c r="A34" s="24">
         <v>17</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -4333,7 +4333,7 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="22"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
         <v>6</v>
@@ -4355,7 +4355,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="22"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
         <v>6</v>
@@ -4401,7 +4401,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="22">
+      <c r="A38" s="24">
         <v>19</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -4427,7 +4427,7 @@
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="22"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
         <v>6</v>
@@ -4449,7 +4449,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="22"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
         <v>6</v>
@@ -4495,7 +4495,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="22">
+      <c r="A42" s="24">
         <v>21</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -4521,7 +4521,7 @@
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="22"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
         <v>6</v>
@@ -4543,7 +4543,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="22"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
         <v>6</v>
@@ -4589,7 +4589,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="22">
+      <c r="A46" s="24">
         <v>23</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -4615,7 +4615,7 @@
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="22"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="s">
         <v>6</v>
@@ -4637,7 +4637,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="22"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6" t="s">
         <v>6</v>
@@ -4683,7 +4683,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="22">
+      <c r="A50" s="24">
         <v>25</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -4709,7 +4709,7 @@
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="22"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
         <v>6</v>
@@ -4731,7 +4731,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="22"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
         <v>6</v>
@@ -4777,7 +4777,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="22">
+      <c r="A54" s="24">
         <v>27</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -4803,7 +4803,7 @@
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="22"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
         <v>6</v>
@@ -4825,7 +4825,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
         <v>6</v>
@@ -4873,7 +4873,7 @@
       <c r="I57" s="17"/>
     </row>
     <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="22">
+      <c r="A58" s="24">
         <v>29</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -4898,7 +4898,7 @@
       <c r="I58" s="5"/>
     </row>
     <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="22"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
         <v>6</v>
@@ -4920,7 +4920,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="22"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
         <v>6</v>
@@ -4967,7 +4967,7 @@
       <c r="I61" s="17"/>
     </row>
     <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="22">
+      <c r="A62" s="24">
         <v>31</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -4993,7 +4993,7 @@
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="22"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
         <v>6</v>
@@ -5015,7 +5015,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="22"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
         <v>6</v>
@@ -5063,7 +5063,7 @@
       <c r="I65" s="17"/>
     </row>
     <row r="66" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="22">
+      <c r="A66" s="24">
         <v>33</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -5089,7 +5089,7 @@
       <c r="I66" s="5"/>
     </row>
     <row r="67" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="22"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
         <v>6</v>
@@ -5111,7 +5111,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="22"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="s">
         <v>6</v>
@@ -5159,7 +5159,7 @@
       <c r="I69" s="17"/>
     </row>
     <row r="70" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="22">
+      <c r="A70" s="24">
         <v>35</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -5185,7 +5185,7 @@
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="22"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
         <v>6</v>
@@ -5207,7 +5207,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="22"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
         <v>6</v>
@@ -5255,7 +5255,7 @@
       <c r="I73" s="17"/>
     </row>
     <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="22">
+      <c r="A74" s="24">
         <v>37</v>
       </c>
       <c r="B74" s="5" t="s">
@@ -5281,7 +5281,7 @@
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="22"/>
+      <c r="A75" s="24"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="s">
         <v>6</v>
@@ -5303,7 +5303,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="22"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6" t="s">
         <v>6</v>
@@ -5351,7 +5351,7 @@
       <c r="I77" s="17"/>
     </row>
     <row r="78" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="22">
+      <c r="A78" s="24">
         <v>39</v>
       </c>
       <c r="B78" s="5" t="s">
@@ -5377,7 +5377,7 @@
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="22"/>
+      <c r="A79" s="24"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
         <v>6</v>
@@ -5399,7 +5399,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="22"/>
+      <c r="A80" s="24"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
         <v>6</v>
@@ -5447,7 +5447,7 @@
       <c r="I81" s="17"/>
     </row>
     <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="22">
+      <c r="A82" s="24">
         <v>41</v>
       </c>
       <c r="B82" s="5" t="s">
@@ -5473,7 +5473,7 @@
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="22"/>
+      <c r="A83" s="24"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6" t="s">
         <v>6</v>
@@ -5495,7 +5495,7 @@
       </c>
     </row>
     <row r="84" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="22"/>
+      <c r="A84" s="24"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6" t="s">
         <v>6</v>
@@ -5543,7 +5543,7 @@
       <c r="I85" s="17"/>
     </row>
     <row r="86" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="22">
+      <c r="A86" s="24">
         <v>43</v>
       </c>
       <c r="B86" s="5" t="s">
@@ -5569,7 +5569,7 @@
       <c r="I86" s="5"/>
     </row>
     <row r="87" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="22"/>
+      <c r="A87" s="24"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6" t="s">
         <v>6</v>
@@ -5591,7 +5591,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="22"/>
+      <c r="A88" s="24"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
         <v>6</v>
@@ -5639,7 +5639,7 @@
       <c r="I89" s="17"/>
     </row>
     <row r="90" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="22">
+      <c r="A90" s="24">
         <v>45</v>
       </c>
       <c r="B90" s="5" t="s">
@@ -5665,7 +5665,7 @@
       <c r="I90" s="5"/>
     </row>
     <row r="91" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="22"/>
+      <c r="A91" s="24"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
         <v>6</v>
@@ -5687,7 +5687,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="22"/>
+      <c r="A92" s="24"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
         <v>6</v>
@@ -5735,7 +5735,7 @@
       <c r="I93" s="17"/>
     </row>
     <row r="94" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="22">
+      <c r="A94" s="24">
         <v>47</v>
       </c>
       <c r="B94" s="5" t="s">
@@ -5761,7 +5761,7 @@
       <c r="I94" s="5"/>
     </row>
     <row r="95" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="22"/>
+      <c r="A95" s="24"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6" t="s">
         <v>6</v>
@@ -5783,7 +5783,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="22"/>
+      <c r="A96" s="24"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6" t="s">
         <v>6</v>
@@ -5831,7 +5831,7 @@
       <c r="I97" s="17"/>
     </row>
     <row r="98" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="22">
+      <c r="A98" s="24">
         <v>49</v>
       </c>
       <c r="B98" s="5" t="s">
@@ -5857,7 +5857,7 @@
       <c r="I98" s="5"/>
     </row>
     <row r="99" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="22"/>
+      <c r="A99" s="24"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6" t="s">
         <v>6</v>
@@ -5879,7 +5879,7 @@
       </c>
     </row>
     <row r="100" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="22"/>
+      <c r="A100" s="24"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6" t="s">
         <v>6</v>
@@ -5927,7 +5927,7 @@
       <c r="I101" s="17"/>
     </row>
     <row r="102" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="22">
+      <c r="A102" s="24">
         <v>51</v>
       </c>
       <c r="B102" s="5" t="s">
@@ -5953,7 +5953,7 @@
       <c r="I102" s="5"/>
     </row>
     <row r="103" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="22"/>
+      <c r="A103" s="24"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6" t="s">
         <v>6</v>
@@ -5975,7 +5975,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="22"/>
+      <c r="A104" s="24"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6" t="s">
         <v>6</v>
@@ -6023,7 +6023,7 @@
       <c r="I105" s="17"/>
     </row>
     <row r="106" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="22">
+      <c r="A106" s="24">
         <v>53</v>
       </c>
       <c r="B106" s="5" t="s">
@@ -6049,7 +6049,7 @@
       <c r="I106" s="5"/>
     </row>
     <row r="107" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" s="22"/>
+      <c r="A107" s="24"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6" t="s">
         <v>6</v>
@@ -6071,7 +6071,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" s="22"/>
+      <c r="A108" s="24"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6" t="s">
         <v>6</v>
@@ -6119,7 +6119,7 @@
       <c r="I109" s="17"/>
     </row>
     <row r="110" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="22">
+      <c r="A110" s="24">
         <v>55</v>
       </c>
       <c r="B110" s="5" t="s">
@@ -6145,7 +6145,7 @@
       <c r="I110" s="5"/>
     </row>
     <row r="111" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="22"/>
+      <c r="A111" s="24"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6" t="s">
         <v>6</v>
@@ -6167,7 +6167,7 @@
       </c>
     </row>
     <row r="112" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="22"/>
+      <c r="A112" s="24"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6" t="s">
         <v>6</v>
@@ -6227,13 +6227,13 @@
       <c r="D114" t="s">
         <v>46</v>
       </c>
-      <c r="E114" s="24">
-        <v>0.01</v>
+      <c r="E114" s="23">
+        <v>1E-3</v>
       </c>
       <c r="F114" t="s">
         <v>24</v>
       </c>
-      <c r="G114" s="23" t="s">
+      <c r="G114" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6250,13 +6250,14 @@
       <c r="D115" t="s">
         <v>47</v>
       </c>
-      <c r="E115" s="24">
-        <v>0.01</v>
+      <c r="E115" s="23">
+        <f>E114*1.4</f>
+        <v>1.4E-3</v>
       </c>
       <c r="F115" t="s">
         <v>24</v>
       </c>
-      <c r="G115" s="23" t="s">
+      <c r="G115" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6273,13 +6274,14 @@
       <c r="D116" t="s">
         <v>48</v>
       </c>
-      <c r="E116" s="24">
-        <v>0.01</v>
+      <c r="E116" s="23">
+        <f t="shared" ref="E116:E128" si="0">E115*1.4</f>
+        <v>1.9599999999999999E-3</v>
       </c>
       <c r="F116" t="s">
         <v>24</v>
       </c>
-      <c r="G116" s="23" t="s">
+      <c r="G116" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6296,13 +6298,14 @@
       <c r="D117" t="s">
         <v>49</v>
       </c>
-      <c r="E117" s="24">
-        <v>0.01</v>
+      <c r="E117" s="23">
+        <f t="shared" si="0"/>
+        <v>2.7439999999999999E-3</v>
       </c>
       <c r="F117" t="s">
         <v>24</v>
       </c>
-      <c r="G117" s="23" t="s">
+      <c r="G117" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6319,13 +6322,14 @@
       <c r="D118" t="s">
         <v>50</v>
       </c>
-      <c r="E118" s="24">
-        <v>0.01</v>
+      <c r="E118" s="23">
+        <f t="shared" si="0"/>
+        <v>3.8415999999999997E-3</v>
       </c>
       <c r="F118" t="s">
         <v>24</v>
       </c>
-      <c r="G118" s="23" t="s">
+      <c r="G118" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6342,13 +6346,14 @@
       <c r="D119" t="s">
         <v>51</v>
       </c>
-      <c r="E119" s="24">
-        <v>0.01</v>
+      <c r="E119" s="23">
+        <f t="shared" si="0"/>
+        <v>5.3782399999999994E-3</v>
       </c>
       <c r="F119" t="s">
         <v>24</v>
       </c>
-      <c r="G119" s="23" t="s">
+      <c r="G119" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6365,13 +6370,14 @@
       <c r="D120" t="s">
         <v>52</v>
       </c>
-      <c r="E120" s="24">
-        <v>0.01</v>
+      <c r="E120" s="23">
+        <f t="shared" si="0"/>
+        <v>7.529535999999999E-3</v>
       </c>
       <c r="F120" t="s">
         <v>24</v>
       </c>
-      <c r="G120" s="23" t="s">
+      <c r="G120" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6388,13 +6394,14 @@
       <c r="D121" t="s">
         <v>53</v>
       </c>
-      <c r="E121" s="24">
-        <v>0.01</v>
+      <c r="E121" s="23">
+        <f t="shared" si="0"/>
+        <v>1.0541350399999998E-2</v>
       </c>
       <c r="F121" t="s">
         <v>24</v>
       </c>
-      <c r="G121" s="23" t="s">
+      <c r="G121" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6411,13 +6418,14 @@
       <c r="D122" t="s">
         <v>54</v>
       </c>
-      <c r="E122" s="24">
-        <v>0.01</v>
+      <c r="E122" s="23">
+        <f t="shared" si="0"/>
+        <v>1.4757890559999997E-2</v>
       </c>
       <c r="F122" t="s">
         <v>24</v>
       </c>
-      <c r="G122" s="23" t="s">
+      <c r="G122" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6434,13 +6442,14 @@
       <c r="D123" t="s">
         <v>55</v>
       </c>
-      <c r="E123" s="24">
-        <v>0.01</v>
+      <c r="E123" s="23">
+        <f t="shared" si="0"/>
+        <v>2.0661046783999996E-2</v>
       </c>
       <c r="F123" t="s">
         <v>24</v>
       </c>
-      <c r="G123" s="23" t="s">
+      <c r="G123" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6457,13 +6466,14 @@
       <c r="D124" t="s">
         <v>56</v>
       </c>
-      <c r="E124" s="24">
-        <v>0.01</v>
+      <c r="E124" s="23">
+        <f t="shared" si="0"/>
+        <v>2.8925465497599993E-2</v>
       </c>
       <c r="F124" t="s">
         <v>24</v>
       </c>
-      <c r="G124" s="23" t="s">
+      <c r="G124" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6480,13 +6490,14 @@
       <c r="D125" t="s">
         <v>57</v>
       </c>
-      <c r="E125" s="24">
-        <v>0.01</v>
+      <c r="E125" s="23">
+        <f t="shared" si="0"/>
+        <v>4.0495651696639989E-2</v>
       </c>
       <c r="F125" t="s">
         <v>24</v>
       </c>
-      <c r="G125" s="23" t="s">
+      <c r="G125" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6503,13 +6514,14 @@
       <c r="D126" t="s">
         <v>58</v>
       </c>
-      <c r="E126" s="24">
-        <v>0.01</v>
+      <c r="E126" s="23">
+        <f t="shared" si="0"/>
+        <v>5.6693912375295981E-2</v>
       </c>
       <c r="F126" t="s">
         <v>24</v>
       </c>
-      <c r="G126" s="23" t="s">
+      <c r="G126" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6526,13 +6538,14 @@
       <c r="D127" t="s">
         <v>59</v>
       </c>
-      <c r="E127" s="24">
-        <v>0.01</v>
+      <c r="E127" s="23">
+        <f t="shared" si="0"/>
+        <v>7.9371477325414372E-2</v>
       </c>
       <c r="F127" t="s">
         <v>24</v>
       </c>
-      <c r="G127" s="23" t="s">
+      <c r="G127" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6549,13 +6562,14 @@
       <c r="D128" t="s">
         <v>60</v>
       </c>
-      <c r="E128" s="24">
-        <v>0.01</v>
+      <c r="E128" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11112006825558012</v>
       </c>
       <c r="F128" t="s">
         <v>24</v>
       </c>
-      <c r="G128" s="23" t="s">
+      <c r="G128" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -7269,7 +7283,7 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="22">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -7294,7 +7308,7 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="22"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -7316,7 +7330,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -7361,7 +7375,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="24">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -7387,7 +7401,7 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -7409,7 +7423,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -7455,7 +7469,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="22">
+      <c r="A10" s="24">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -7481,7 +7495,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="22"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>6</v>
@@ -7503,7 +7517,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="22"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>6</v>
@@ -7549,7 +7563,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
+      <c r="A14" s="24">
         <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -7575,7 +7589,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="22"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
         <v>6</v>
@@ -7597,7 +7611,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="22"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>6</v>
@@ -7643,7 +7657,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="22">
+      <c r="A18" s="24">
         <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -7669,7 +7683,7 @@
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="22"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>6</v>
@@ -7691,7 +7705,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="22"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
         <v>6</v>
@@ -7737,7 +7751,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="22">
+      <c r="A22" s="24">
         <v>11</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -7763,7 +7777,7 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="22"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="s">
         <v>6</v>
@@ -7785,7 +7799,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="22"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
         <v>6</v>
@@ -7831,7 +7845,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="22">
+      <c r="A26" s="24">
         <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -7857,7 +7871,7 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="22"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>6</v>
@@ -7879,7 +7893,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="22"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
         <v>6</v>
@@ -7925,7 +7939,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="22">
+      <c r="A30" s="24">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -7950,7 +7964,7 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="22"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
         <v>6</v>
@@ -7972,7 +7986,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="22"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
         <v>6</v>
@@ -8018,7 +8032,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="22">
+      <c r="A34" s="24">
         <v>17</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -8043,7 +8057,7 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="22"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
         <v>6</v>
@@ -8065,7 +8079,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="22"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
         <v>6</v>
@@ -8111,7 +8125,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="22">
+      <c r="A38" s="24">
         <v>19</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -8136,7 +8150,7 @@
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="22"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
         <v>6</v>
@@ -8158,7 +8172,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="22"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
         <v>6</v>
@@ -8204,7 +8218,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="22">
+      <c r="A42" s="24">
         <v>21</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -8229,7 +8243,7 @@
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="22"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
         <v>6</v>
@@ -8251,7 +8265,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="22"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
         <v>6</v>
@@ -8297,7 +8311,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="22">
+      <c r="A46" s="24">
         <v>23</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -8322,7 +8336,7 @@
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="22"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="s">
         <v>6</v>
@@ -8344,7 +8358,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="22"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6" t="s">
         <v>6</v>
@@ -8390,7 +8404,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="22">
+      <c r="A50" s="24">
         <v>25</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -8415,7 +8429,7 @@
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="22"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
         <v>6</v>
@@ -8437,7 +8451,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="22"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
         <v>6</v>
@@ -8483,7 +8497,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="22">
+      <c r="A54" s="24">
         <v>27</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -8508,7 +8522,7 @@
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="22"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
         <v>6</v>
@@ -8530,7 +8544,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="22"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
         <v>6</v>
@@ -8646,287 +8660,287 @@
     <mergeCell ref="A18:A20"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:D2 C5:D5 C9 C13 C17 C21 C25 C29 C33 C37 C41 C45 C49 C53 C57">
-    <cfRule type="expression" dxfId="70" priority="56">
+    <cfRule type="expression" dxfId="69" priority="56">
       <formula>ISODD($K2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D2">
-    <cfRule type="expression" dxfId="69" priority="57">
+    <cfRule type="expression" dxfId="68" priority="57">
       <formula>ISODD($K2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:I4 B58:I58 B60:I61 E7:I8 E11:I12 E15:I16 E19:I20 E23:I24 E27:I28 E31:I32 E35:I36 E39:I40 E43:I44 E47:I48 E51:I52 E55:I56">
-    <cfRule type="expression" dxfId="68" priority="55">
+    <cfRule type="expression" dxfId="67" priority="55">
       <formula>ISODD($I3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:D59">
-    <cfRule type="expression" dxfId="67" priority="53">
+    <cfRule type="expression" dxfId="66" priority="53">
       <formula>ISODD($K59)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:D59">
-    <cfRule type="expression" dxfId="66" priority="54">
+    <cfRule type="expression" dxfId="65" priority="54">
       <formula>ISODD($K59)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="65" priority="51">
+    <cfRule type="expression" dxfId="64" priority="51">
       <formula>ISODD($K6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="64" priority="52">
+    <cfRule type="expression" dxfId="63" priority="52">
       <formula>ISODD($K6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:C8">
-    <cfRule type="expression" dxfId="63" priority="50">
+    <cfRule type="expression" dxfId="62" priority="50">
       <formula>ISODD($I7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="62" priority="48">
+    <cfRule type="expression" dxfId="61" priority="48">
       <formula>ISODD($K10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="61" priority="49">
+    <cfRule type="expression" dxfId="60" priority="49">
       <formula>ISODD($K10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C12">
-    <cfRule type="expression" dxfId="60" priority="47">
+    <cfRule type="expression" dxfId="59" priority="47">
       <formula>ISODD($I11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="59" priority="45">
+    <cfRule type="expression" dxfId="58" priority="45">
       <formula>ISODD($K14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="58" priority="46">
+    <cfRule type="expression" dxfId="57" priority="46">
       <formula>ISODD($K14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:C16">
-    <cfRule type="expression" dxfId="57" priority="44">
+    <cfRule type="expression" dxfId="56" priority="44">
       <formula>ISODD($I15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="56" priority="42">
+    <cfRule type="expression" dxfId="55" priority="42">
       <formula>ISODD($K18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="55" priority="43">
+    <cfRule type="expression" dxfId="54" priority="43">
       <formula>ISODD($K18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:C20">
-    <cfRule type="expression" dxfId="54" priority="41">
+    <cfRule type="expression" dxfId="53" priority="41">
       <formula>ISODD($I19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="53" priority="39">
+    <cfRule type="expression" dxfId="52" priority="39">
       <formula>ISODD($K22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="52" priority="40">
+    <cfRule type="expression" dxfId="51" priority="40">
       <formula>ISODD($K22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C24">
-    <cfRule type="expression" dxfId="51" priority="38">
+    <cfRule type="expression" dxfId="50" priority="38">
       <formula>ISODD($I23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="50" priority="36">
+    <cfRule type="expression" dxfId="49" priority="36">
       <formula>ISODD($K26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="49" priority="37">
+    <cfRule type="expression" dxfId="48" priority="37">
       <formula>ISODD($K26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C28">
-    <cfRule type="expression" dxfId="48" priority="35">
+    <cfRule type="expression" dxfId="47" priority="35">
       <formula>ISODD($I27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="47" priority="33">
+    <cfRule type="expression" dxfId="46" priority="33">
       <formula>ISODD($K30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="46" priority="34">
+    <cfRule type="expression" dxfId="45" priority="34">
       <formula>ISODD($K30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:C32">
-    <cfRule type="expression" dxfId="45" priority="32">
+    <cfRule type="expression" dxfId="44" priority="32">
       <formula>ISODD($I31)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="44" priority="30">
+    <cfRule type="expression" dxfId="43" priority="30">
       <formula>ISODD($K34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="43" priority="31">
+    <cfRule type="expression" dxfId="42" priority="31">
       <formula>ISODD($K34)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:C36">
-    <cfRule type="expression" dxfId="42" priority="29">
+    <cfRule type="expression" dxfId="41" priority="29">
       <formula>ISODD($I35)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="41" priority="27">
+    <cfRule type="expression" dxfId="40" priority="27">
       <formula>ISODD($K38)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="40" priority="28">
+    <cfRule type="expression" dxfId="39" priority="28">
       <formula>ISODD($K38)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:C40">
-    <cfRule type="expression" dxfId="39" priority="26">
+    <cfRule type="expression" dxfId="38" priority="26">
       <formula>ISODD($I39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="38" priority="24">
+    <cfRule type="expression" dxfId="37" priority="24">
       <formula>ISODD($K42)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="37" priority="25">
+    <cfRule type="expression" dxfId="36" priority="25">
       <formula>ISODD($K42)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:C44">
-    <cfRule type="expression" dxfId="36" priority="23">
+    <cfRule type="expression" dxfId="35" priority="23">
       <formula>ISODD($I43)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="35" priority="21">
+    <cfRule type="expression" dxfId="34" priority="21">
       <formula>ISODD($K46)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="34" priority="22">
+    <cfRule type="expression" dxfId="33" priority="22">
       <formula>ISODD($K46)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:C48">
-    <cfRule type="expression" dxfId="33" priority="20">
+    <cfRule type="expression" dxfId="32" priority="20">
       <formula>ISODD($I47)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="32" priority="18">
+    <cfRule type="expression" dxfId="31" priority="18">
       <formula>ISODD($K50)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="31" priority="19">
+    <cfRule type="expression" dxfId="30" priority="19">
       <formula>ISODD($K50)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:C52">
-    <cfRule type="expression" dxfId="30" priority="17">
+    <cfRule type="expression" dxfId="29" priority="17">
       <formula>ISODD($I51)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8">
-    <cfRule type="expression" dxfId="29" priority="16">
+    <cfRule type="expression" dxfId="28" priority="16">
       <formula>ISODD($I7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D12">
-    <cfRule type="expression" dxfId="28" priority="15">
+    <cfRule type="expression" dxfId="27" priority="15">
       <formula>ISODD($I11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D16">
-    <cfRule type="expression" dxfId="27" priority="14">
+    <cfRule type="expression" dxfId="26" priority="14">
       <formula>ISODD($I15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:D20">
-    <cfRule type="expression" dxfId="26" priority="13">
+    <cfRule type="expression" dxfId="25" priority="13">
       <formula>ISODD($I19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="expression" dxfId="25" priority="12">
+    <cfRule type="expression" dxfId="24" priority="12">
       <formula>ISODD($I23)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D28">
-    <cfRule type="expression" dxfId="24" priority="11">
+    <cfRule type="expression" dxfId="23" priority="11">
       <formula>ISODD($I27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D32">
-    <cfRule type="expression" dxfId="23" priority="10">
+    <cfRule type="expression" dxfId="22" priority="10">
       <formula>ISODD($I31)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D36">
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>ISODD($I35)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:D40">
-    <cfRule type="expression" dxfId="21" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>ISODD($I39)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D44">
-    <cfRule type="expression" dxfId="20" priority="7">
+    <cfRule type="expression" dxfId="19" priority="7">
       <formula>ISODD($I43)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47:D48">
-    <cfRule type="expression" dxfId="19" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>ISODD($I47)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D52">
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="17" priority="5">
       <formula>ISODD($I51)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>ISODD($K54)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>ISODD($K54)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:C56">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>ISODD($I55)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:D56">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>ISODD($I55)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9039,7 +9053,7 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="22">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -9064,7 +9078,7 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="22"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -9086,7 +9100,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -9131,7 +9145,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="24">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -9157,7 +9171,7 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -9179,7 +9193,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -9225,7 +9239,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="22">
+      <c r="A10" s="24">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -9251,7 +9265,7 @@
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="22"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>6</v>
@@ -9273,7 +9287,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="22"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6" t="s">
         <v>6</v>
@@ -9369,67 +9383,67 @@
     <mergeCell ref="A10:A12"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:D2 C5:D5 C9 C13">
-    <cfRule type="expression" dxfId="13" priority="110">
+    <cfRule type="expression" dxfId="12" priority="110">
       <formula>ISODD($K2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D2">
-    <cfRule type="expression" dxfId="12" priority="111">
+    <cfRule type="expression" dxfId="11" priority="111">
       <formula>ISODD($K2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:I4 B14:I14 B16:I17 E7:I8 E11:I12">
-    <cfRule type="expression" dxfId="11" priority="107">
+    <cfRule type="expression" dxfId="10" priority="107">
       <formula>ISODD($I3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:D15">
-    <cfRule type="expression" dxfId="10" priority="72">
+    <cfRule type="expression" dxfId="9" priority="72">
       <formula>ISODD($K15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:D15">
-    <cfRule type="expression" dxfId="9" priority="73">
+    <cfRule type="expression" dxfId="8" priority="73">
       <formula>ISODD($K15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="8" priority="68">
+    <cfRule type="expression" dxfId="7" priority="68">
       <formula>ISODD($K6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="7" priority="69">
+    <cfRule type="expression" dxfId="6" priority="69">
       <formula>ISODD($K6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:C8">
-    <cfRule type="expression" dxfId="6" priority="67">
+    <cfRule type="expression" dxfId="5" priority="67">
       <formula>ISODD($I7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="5" priority="65">
+    <cfRule type="expression" dxfId="4" priority="65">
       <formula>ISODD($K10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="4" priority="66">
+    <cfRule type="expression" dxfId="3" priority="66">
       <formula>ISODD($K10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:C12">
-    <cfRule type="expression" dxfId="3" priority="64">
+    <cfRule type="expression" dxfId="2" priority="64">
       <formula>ISODD($I11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8">
-    <cfRule type="expression" dxfId="2" priority="30">
+    <cfRule type="expression" dxfId="1" priority="30">
       <formula>ISODD($I7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D12">
-    <cfRule type="expression" dxfId="1" priority="29">
+    <cfRule type="expression" dxfId="0" priority="29">
       <formula>ISODD($I11)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>